<commit_message>
changes to evaluation metrics fal_neg_rate and tru_pos_rate
</commit_message>
<xml_diff>
--- a/data/wyniki.xlsx
+++ b/data/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakubkozlowski/Documents/Studia/Semestr2/data_mining/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8846B3DF-20FC-ED43-BF84-076810B6367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32FF04-4E7B-2A47-9893-88561157C44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,12 +454,13 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="M11" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
         <v>2.6969108467983172E-2</v>
       </c>
       <c r="L2">
-        <v>7.0921985815602842E-4</v>
+        <v>1.5278462296697879E-2</v>
       </c>
       <c r="M2">
         <v>4.5710363761153047E-2</v>
@@ -580,7 +580,7 @@
         <v>6.0520842377832507E-3</v>
       </c>
       <c r="L3">
-        <v>2.2420498741706702E-3</v>
+        <v>4.8299655002464269E-2</v>
       </c>
       <c r="M3">
         <v>4.4177533745138407E-2</v>
@@ -621,7 +621,7 @@
         <v>2.6017965524399722E-3</v>
       </c>
       <c r="L4">
-        <v>2.2878059940517051E-3</v>
+        <v>4.928536224741252E-2</v>
       </c>
       <c r="M4">
         <v>4.4131777625257378E-2</v>
@@ -662,7 +662,7 @@
         <v>6.7165933424574775E-2</v>
       </c>
       <c r="L5">
-        <v>5.0789293067947834E-3</v>
+        <v>0.1094135041892558</v>
       </c>
       <c r="M5">
         <v>4.1340654312514297E-2</v>
@@ -703,7 +703,7 @@
         <v>7.9980127608902052E-2</v>
       </c>
       <c r="L6">
-        <v>5.6737588652482273E-3</v>
+        <v>0.12222769837358299</v>
       </c>
       <c r="M6">
         <v>4.0745824754060862E-2</v>
@@ -744,7 +744,7 @@
         <v>0.10511566235508241</v>
       </c>
       <c r="L7">
-        <v>6.840539922214596E-3</v>
+        <v>0.1473632331197634</v>
       </c>
       <c r="M7">
         <v>3.9579043697094488E-2</v>
@@ -785,7 +785,7 @@
         <v>0.12581520217097131</v>
       </c>
       <c r="L8">
-        <v>8.0073209791809655E-3</v>
+        <v>0.17249876786594379</v>
       </c>
       <c r="M8">
         <v>3.841226264012812E-2</v>
@@ -826,7 +826,7 @@
         <v>0.12827947028334191</v>
       </c>
       <c r="L9">
-        <v>8.1217112788835501E-3</v>
+        <v>0.17496303597831439</v>
       </c>
       <c r="M9">
         <v>3.8297872340425532E-2</v>
@@ -867,7 +867,7 @@
         <v>0.16130066298910831</v>
       </c>
       <c r="L10">
-        <v>9.6545412948981918E-3</v>
+        <v>0.20798422868408081</v>
       </c>
       <c r="M10">
         <v>3.6765042324410892E-2</v>
@@ -908,7 +908,7 @@
         <v>0.25789997299403677</v>
       </c>
       <c r="L11">
-        <v>1.413864104323953E-2</v>
+        <v>0.30458353868900928</v>
       </c>
       <c r="M11">
         <v>3.2280942576069553E-2</v>

</xml_diff>